<commit_message>
updated template of students
</commit_message>
<xml_diff>
--- a/public/docs/Шаблон_Окуучу.xlsx
+++ b/public/docs/Шаблон_Окуучу.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t xml:space="preserve">Окуучу</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">ПИН</t>
   </si>
   <si>
-    <t xml:space="preserve">Классы</t>
+    <t xml:space="preserve">Класс</t>
   </si>
   <si>
     <t xml:space="preserve">Бөлүм</t>
@@ -79,6 +79,9 @@
     <t xml:space="preserve">E</t>
   </si>
   <si>
+    <t xml:space="preserve">11.02.1996</t>
+  </si>
+  <si>
     <t xml:space="preserve">ул. Патриса 64кв20</t>
   </si>
   <si>
@@ -103,6 +106,9 @@
     <t xml:space="preserve">Адалбеков</t>
   </si>
   <si>
+    <t xml:space="preserve">05.10.1995</t>
+  </si>
+  <si>
     <t xml:space="preserve">Жер-Ынтымак 62</t>
   </si>
   <si>
@@ -130,6 +136,9 @@
     <t xml:space="preserve">Дамиров</t>
   </si>
   <si>
+    <t xml:space="preserve">08.11.1995</t>
+  </si>
+  <si>
     <t xml:space="preserve">ж/м Ала-Тоо ул. Ала-Тоо 79</t>
   </si>
   <si>
@@ -149,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">Съезбеков</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.09.1996</t>
   </si>
   <si>
     <t xml:space="preserve">ж/м Алтын-Ордо 458</t>
@@ -173,10 +185,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="DD\.MM\.YYYY"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -312,7 +323,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -345,10 +356,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -362,10 +369,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -453,27 +456,27 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.2429149797571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -555,7 +558,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
@@ -577,193 +580,193 @@
       <c r="G3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="8" t="n">
-        <v>40596</v>
+      <c r="H3" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M3" s="6" t="n">
         <v>700884657</v>
       </c>
       <c r="N3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="Q3" s="6" t="n">
         <v>705711811</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="n">
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="11" t="n">
+      <c r="E4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="13" t="n">
-        <v>40839</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="12" t="s">
+      <c r="H4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="14" t="n">
+      <c r="K4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="12" t="n">
         <v>559638217</v>
       </c>
-      <c r="N4" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" s="12" t="s">
+      <c r="N4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Q4" s="14" t="n">
+      <c r="O4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="12" t="n">
         <v>703020506</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="n">
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="10" t="n">
+        <v>707489971</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="Q5" s="10" t="n">
+        <v>700791959</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="11" t="n">
+      <c r="E6" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="13" t="n">
-        <v>40735</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" s="12" t="s">
+      <c r="H6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="10" t="n">
+        <v>702071085</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="M5" s="11" t="n">
-        <v>707489971</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q5" s="11" t="n">
-        <v>700791959</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="13" t="n">
-        <v>40544</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M6" s="11" t="n">
-        <v>702071085</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="P6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q6" s="11" t="n">
+      <c r="Q6" s="10" t="n">
         <v>708000741</v>
       </c>
     </row>

</xml_diff>